<commit_message>
graph of files over total files
</commit_message>
<xml_diff>
--- a/OSSprojects/File_commit/filesPerc/Summary of data.xlsx
+++ b/OSSprojects/File_commit/filesPerc/Summary of data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="640" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="560" yWindow="640" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="C++" sheetId="1" r:id="rId1"/>
@@ -334,7 +334,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6330" uniqueCount="886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6331" uniqueCount="886">
   <si>
     <t>cocos2d-x</t>
   </si>
@@ -2998,10 +2998,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3024,15 +3040,131 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="59">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3342,8 +3474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AE47" sqref="AE47"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2:AA54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7978,7 +8110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA57"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="AA2" sqref="AA2:AA57"/>
     </sheetView>
   </sheetViews>
@@ -12871,8 +13003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA77"/>
   <sheetViews>
-    <sheetView topLeftCell="J41" workbookViewId="0">
-      <selection activeCell="AD67" sqref="AD67"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12931,6 +13063,9 @@
       </c>
       <c r="Y1" t="s">
         <v>60</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
@@ -63731,8 +63866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA21"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1:AA1"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2:AA21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -65529,7 +65664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J145" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AD168" sqref="AD168"/>
     </sheetView>
   </sheetViews>

</xml_diff>